<commit_message>
Add Stock Functionality Testing Added
</commit_message>
<xml_diff>
--- a/POMFramework/TestData/RediffTestData.xlsx
+++ b/POMFramework/TestData/RediffTestData.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Testing\POMFramework\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41EE5933-6111-450A-BE4D-9A08E1F9855B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{426248AB-CB5E-4AAA-90EF-CD2E1896901E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{5C3F3F7D-5C13-4130-A947-D0EAFE1E086C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{5C3F3F7D-5C13-4130-A947-D0EAFE1E086C}"/>
   </bookViews>
   <sheets>
     <sheet name="RediffLoginTest" sheetId="1" r:id="rId1"/>
+    <sheet name="StockTestData" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="34">
   <si>
     <t>Portfolio_Credentials</t>
   </si>
@@ -109,6 +110,24 @@
   </si>
   <si>
     <t>Income Portfolio</t>
+  </si>
+  <si>
+    <t>AddStockTest</t>
+  </si>
+  <si>
+    <t>StockName</t>
+  </si>
+  <si>
+    <t>StockQty</t>
+  </si>
+  <si>
+    <t>StockPrice</t>
+  </si>
+  <si>
+    <t>My 2023 Stock</t>
+  </si>
+  <si>
+    <t>ITC</t>
   </si>
 </sst>
 </file>
@@ -487,7 +506,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09CF6C67-BD57-4334-B647-3C84A4E384A7}">
   <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
@@ -650,4 +669,62 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C7B622A-6A90-4560-9B7F-8CF2831F71E1}">
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3">
+        <v>1000</v>
+      </c>
+      <c r="D3">
+        <v>420</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>